<commit_message>
added project schedule and latest version of project proposal
</commit_message>
<xml_diff>
--- a/project_1_schedule.xlsx
+++ b/project_1_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikem\Documents\MDAB-homework\07-project-1-challenge\schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F28762-8D30-4B81-BB1B-44B8FFED2311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0030BD-CBE2-47C7-9FE8-89D42AC9DAE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11580" xr2:uid="{F01955E0-0F83-4BCF-9713-4BEC5107A800}"/>
   </bookViews>
@@ -273,9 +273,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -283,6 +280,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -603,7 +603,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -611,20 +611,20 @@
     <col min="1" max="1" width="8.7265625" style="2"/>
     <col min="2" max="2" width="67.26953125" customWidth="1"/>
     <col min="3" max="4" width="13.81640625" customWidth="1"/>
-    <col min="5" max="5" width="14.54296875" style="16" customWidth="1"/>
+    <col min="5" max="5" width="14.54296875" style="15" customWidth="1"/>
     <col min="6" max="6" width="14.04296875" customWidth="1"/>
     <col min="7" max="7" width="10.2265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A2" s="3" t="s">
@@ -651,7 +651,7 @@
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
-      <c r="E3" s="14"/>
+      <c r="E3" s="13"/>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.75">
@@ -663,7 +663,7 @@
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="14"/>
+      <c r="E4" s="13"/>
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.75">
@@ -676,7 +676,7 @@
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
-      <c r="E5" s="14"/>
+      <c r="E5" s="13"/>
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.75">
@@ -689,7 +689,7 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="14"/>
+      <c r="E6" s="13"/>
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.75">
@@ -702,7 +702,7 @@
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="14"/>
+      <c r="E7" s="13"/>
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.75">
@@ -710,7 +710,7 @@
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
-      <c r="E8" s="14"/>
+      <c r="E8" s="13"/>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.75">
@@ -722,7 +722,7 @@
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
-      <c r="E9" s="14"/>
+      <c r="E9" s="13"/>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.75">
@@ -735,7 +735,7 @@
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
-      <c r="E10" s="14"/>
+      <c r="E10" s="13"/>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="29.5" x14ac:dyDescent="0.75">
@@ -748,7 +748,7 @@
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="14"/>
+      <c r="E11" s="13"/>
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" ht="29.5" x14ac:dyDescent="0.75">
@@ -761,7 +761,7 @@
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="14"/>
+      <c r="E12" s="13"/>
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.75">
@@ -769,7 +769,7 @@
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="14"/>
+      <c r="E13" s="13"/>
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.75">
@@ -781,7 +781,7 @@
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="14"/>
+      <c r="E14" s="13"/>
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.75">
@@ -794,7 +794,7 @@
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
-      <c r="E15" s="14"/>
+      <c r="E15" s="13"/>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.75">
@@ -807,7 +807,7 @@
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="14"/>
+      <c r="E16" s="13"/>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.75">
@@ -815,7 +815,7 @@
       <c r="B17" s="7"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="14"/>
+      <c r="E17" s="13"/>
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.75">
@@ -827,7 +827,7 @@
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
-      <c r="E18" s="14"/>
+      <c r="E18" s="13"/>
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.75">
@@ -840,7 +840,7 @@
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
-      <c r="E19" s="14"/>
+      <c r="E19" s="13"/>
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.75">
@@ -853,7 +853,7 @@
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
-      <c r="E20" s="14"/>
+      <c r="E20" s="13"/>
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.75">
@@ -866,7 +866,7 @@
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="14"/>
+      <c r="E21" s="13"/>
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.75">
@@ -874,7 +874,7 @@
       <c r="B22" s="7"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
-      <c r="E22" s="14"/>
+      <c r="E22" s="13"/>
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.75">
@@ -886,7 +886,7 @@
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
-      <c r="E23" s="14"/>
+      <c r="E23" s="13"/>
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.75">
@@ -899,7 +899,7 @@
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="14"/>
+      <c r="E24" s="13"/>
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.75">
@@ -912,7 +912,7 @@
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
-      <c r="E25" s="14"/>
+      <c r="E25" s="13"/>
       <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.75">
@@ -925,7 +925,7 @@
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
-      <c r="E26" s="14"/>
+      <c r="E26" s="13"/>
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.75">
@@ -933,7 +933,7 @@
       <c r="B27" s="7"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="14"/>
+      <c r="E27" s="13"/>
       <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.75">
@@ -945,7 +945,7 @@
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
-      <c r="E28" s="14"/>
+      <c r="E28" s="13"/>
       <c r="F28" s="5"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.75">
@@ -958,7 +958,7 @@
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
-      <c r="E29" s="14"/>
+      <c r="E29" s="13"/>
       <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.75">
@@ -971,7 +971,7 @@
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="14"/>
+      <c r="E30" s="13"/>
       <c r="F30" s="5"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.75">
@@ -984,7 +984,7 @@
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
-      <c r="E31" s="14"/>
+      <c r="E31" s="13"/>
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.75">
@@ -992,7 +992,7 @@
       <c r="B32" s="6"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
-      <c r="E32" s="14"/>
+      <c r="E32" s="13"/>
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.75">
@@ -1004,7 +1004,7 @@
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
-      <c r="E33" s="14"/>
+      <c r="E33" s="13"/>
       <c r="F33" s="5"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.75">
@@ -1017,7 +1017,7 @@
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
-      <c r="E34" s="14"/>
+      <c r="E34" s="13"/>
       <c r="F34" s="5"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.75">
@@ -1030,7 +1030,7 @@
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
-      <c r="E35" s="14"/>
+      <c r="E35" s="13"/>
       <c r="F35" s="5"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.75">
@@ -1043,7 +1043,7 @@
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
-      <c r="E36" s="14"/>
+      <c r="E36" s="13"/>
       <c r="F36" s="5"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.75">
@@ -1056,7 +1056,7 @@
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
-      <c r="E37" s="14"/>
+      <c r="E37" s="13"/>
       <c r="F37" s="5"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.75">
@@ -1069,7 +1069,7 @@
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
-      <c r="E38" s="14"/>
+      <c r="E38" s="13"/>
       <c r="F38" s="5"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.75">
@@ -1082,7 +1082,7 @@
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
-      <c r="E39" s="14"/>
+      <c r="E39" s="13"/>
       <c r="F39" s="5"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.75">
@@ -1090,7 +1090,7 @@
       <c r="B40" s="6"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
-      <c r="E40" s="14"/>
+      <c r="E40" s="13"/>
       <c r="F40" s="5"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.75">
@@ -1102,7 +1102,7 @@
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
-      <c r="E41" s="14"/>
+      <c r="E41" s="13"/>
       <c r="F41" s="5"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.75">
@@ -1110,7 +1110,7 @@
       <c r="B42" s="6"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
-      <c r="E42" s="14"/>
+      <c r="E42" s="13"/>
       <c r="F42" s="5"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.75">
@@ -1122,7 +1122,7 @@
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
-      <c r="E43" s="14"/>
+      <c r="E43" s="13"/>
       <c r="F43" s="5"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.75">
@@ -1130,7 +1130,7 @@
       <c r="B44" s="6"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
-      <c r="E44" s="14"/>
+      <c r="E44" s="13"/>
       <c r="F44" s="5"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.75">
@@ -1142,7 +1142,7 @@
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
-      <c r="E45" s="14"/>
+      <c r="E45" s="13"/>
       <c r="F45" s="5"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.75">
@@ -1150,7 +1150,7 @@
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
-      <c r="E46" s="14"/>
+      <c r="E46" s="13"/>
       <c r="F46" s="5"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.75">
@@ -1162,7 +1162,7 @@
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
-      <c r="E47" s="14"/>
+      <c r="E47" s="13"/>
       <c r="F47" s="5"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.75">
@@ -1170,7 +1170,7 @@
       <c r="B48" s="6"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
-      <c r="E48" s="14"/>
+      <c r="E48" s="13"/>
       <c r="F48" s="5"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.75">
@@ -1182,7 +1182,7 @@
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
-      <c r="E49" s="14"/>
+      <c r="E49" s="13"/>
       <c r="F49" s="5"/>
     </row>
     <row r="50" spans="1:6" ht="29.5" x14ac:dyDescent="0.75">
@@ -1195,7 +1195,7 @@
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
-      <c r="E50" s="14"/>
+      <c r="E50" s="13"/>
       <c r="F50" s="5"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.75">
@@ -1203,7 +1203,7 @@
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
-      <c r="E51" s="14"/>
+      <c r="E51" s="13"/>
       <c r="F51" s="5"/>
     </row>
     <row r="52" spans="1:6" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
@@ -1211,7 +1211,7 @@
       <c r="B52" s="11"/>
       <c r="C52" s="11"/>
       <c r="D52" s="11"/>
-      <c r="E52" s="15"/>
+      <c r="E52" s="14"/>
       <c r="F52" s="11"/>
     </row>
   </sheetData>

</xml_diff>